<commit_message>
Add folder for knowledge base
</commit_message>
<xml_diff>
--- a/ArticlesNeedManualEfforts.xlsx
+++ b/ArticlesNeedManualEfforts.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>KnowledgeBaseArticles\Accounts\Accounts (UDN)</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>Articles need manual efforts after customization</t>
+  </si>
+  <si>
+    <t>After applying another .net dll (reverse markdown) for conversion of html to md</t>
   </si>
 </sst>
 </file>
@@ -507,15 +510,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1766FF7D-08F3-4DE7-971D-597519344526}">
-  <dimension ref="A2:B44"/>
+  <dimension ref="A2:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="72.7109375" customWidth="1"/>
+    <col min="1" max="1" width="82.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="46.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -815,6 +818,14 @@
         <v>91.3</v>
       </c>
     </row>
+    <row r="46" spans="1:2" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B46" s="1">
+        <v>94.14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>